<commit_message>
Update for sounds and raster text bitmap
Update for sounds and raster text bitmap
</commit_message>
<xml_diff>
--- a/Analysis/SabreWulf/Data/MemoryLayout.xlsx
+++ b/Analysis/SabreWulf/Data/MemoryLayout.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IC514955\Documents\My Developments\FractalStudios\GitHub\ZxSpectrum\Analysis\SabreWulf\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IC514955\Documents\Development\FractalStudios\GitHub\ZxSpectrum\Analysis\SabreWulf\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DE7D20-7375-4FBB-8D8D-A949AD623009}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8615E8C-E2D5-44BF-81DC-D286F1A63C9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="5760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="5760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Default Immortal Moving Objects" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$2:$I$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$2:$I$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="196">
   <si>
     <t>start</t>
   </si>
@@ -129,15 +129,9 @@
     <t>e1ec</t>
   </si>
   <si>
-    <t>969c</t>
-  </si>
-  <si>
     <t>96df</t>
   </si>
   <si>
-    <t>969b</t>
-  </si>
-  <si>
     <t>96de</t>
   </si>
   <si>
@@ -255,9 +249,6 @@
     <t>a2bd</t>
   </si>
   <si>
-    <t>a29b</t>
-  </si>
-  <si>
     <t>a7f8</t>
   </si>
   <si>
@@ -529,6 +520,108 @@
   </si>
   <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>bc66</t>
+  </si>
+  <si>
+    <t>Game Over Tune</t>
+  </si>
+  <si>
+    <t>Amulet Found Tune</t>
+  </si>
+  <si>
+    <t>Start Game Tune</t>
+  </si>
+  <si>
+    <t>Frequency Table</t>
+  </si>
+  <si>
+    <t>bdd2</t>
+  </si>
+  <si>
+    <t>bc67</t>
+  </si>
+  <si>
+    <t>bd28</t>
+  </si>
+  <si>
+    <t>bd32</t>
+  </si>
+  <si>
+    <t>bd33</t>
+  </si>
+  <si>
+    <t>bd45</t>
+  </si>
+  <si>
+    <t>bd44</t>
+  </si>
+  <si>
+    <t>bd50</t>
+  </si>
+  <si>
+    <t>bd51</t>
+  </si>
+  <si>
+    <t>Code (Play sounds)</t>
+  </si>
+  <si>
+    <t>bdd1</t>
+  </si>
+  <si>
+    <t>bec5</t>
+  </si>
+  <si>
+    <t>bec6</t>
+  </si>
+  <si>
+    <t>becb</t>
+  </si>
+  <si>
+    <t>becc</t>
+  </si>
+  <si>
+    <t>bedd</t>
+  </si>
+  <si>
+    <t>bede</t>
+  </si>
+  <si>
+    <t>bf07</t>
+  </si>
+  <si>
+    <t>bf08</t>
+  </si>
+  <si>
+    <t>96bc</t>
+  </si>
+  <si>
+    <t>96bb</t>
+  </si>
+  <si>
+    <t>Jump Table</t>
+  </si>
+  <si>
+    <t>9b3e</t>
+  </si>
+  <si>
+    <t>9cc5</t>
+  </si>
+  <si>
+    <t>9cc6</t>
+  </si>
+  <si>
+    <t>9b3d</t>
+  </si>
+  <si>
+    <t>a29c</t>
+  </si>
+  <si>
+    <t>bd27</t>
+  </si>
+  <si>
+    <t>Game Start/Completed Tune</t>
   </si>
 </sst>
 </file>
@@ -911,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q62"/>
+  <dimension ref="A2:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,23 +1050,23 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
-        <f>SUM(C4:C58)</f>
+        <f>SUM(C4:C70)</f>
         <v>65536</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C4" s="2">
         <f>HEX2DEC(B4)-HEX2DEC(A4)+1</f>
         <v>16384</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -981,14 +1074,14 @@
         <v>4000</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ref="C5:C7" si="0">HEX2DEC(B5)-HEX2DEC(A5)+1</f>
         <v>6144</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -996,45 +1089,45 @@
         <v>5800</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>768</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H6" s="2">
-        <f>SUM(H7:H58)</f>
-        <v>42226</v>
+        <f>SUM(H7:H70)</f>
+        <v>42227</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" ref="H7:H45" si="1">HEX2DEC(G7)-HEX2DEC(F7)+1</f>
+        <f t="shared" ref="H7:H57" si="1">HEX2DEC(G7)-HEX2DEC(F7)+1</f>
         <v>13</v>
       </c>
       <c r="I7" s="2">
@@ -1044,13 +1137,13 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="1"/>
@@ -1061,28 +1154,28 @@
         <v>128</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2">
         <f>HEX2DEC(B9)-HEX2DEC(A9)+1</f>
         <v>192</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>5</v>
@@ -1098,7 +1191,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>6</v>
@@ -1117,26 +1210,26 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C11" s="2">
         <f>HEX2DEC(B11)-HEX2DEC(A11)+1</f>
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="2"/>
@@ -1149,20 +1242,20 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2">
         <f>HEX2DEC(B12)-HEX2DEC(A12)+1</f>
         <v>41613</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>8</v>
@@ -1176,12 +1269,12 @@
         <v>1152</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F13" s="5">
         <v>6000</v>
@@ -1200,7 +1293,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F14" s="5">
         <v>6007</v>
@@ -1219,7 +1312,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E15" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F15" s="6">
         <v>6036</v>
@@ -1336,42 +1429,42 @@
         <v>9692</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>33</v>
+        <v>187</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="4"/>
-        <v>15132</v>
+        <v>15164</v>
       </c>
       <c r="K21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F22" s="5" t="s">
-        <v>31</v>
+        <v>186</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="4"/>
         <v>15199</v>
       </c>
       <c r="K22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" s="5">
         <v>9701</v>
@@ -1385,12 +1478,12 @@
         <v>15234</v>
       </c>
       <c r="K23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F24" s="5">
         <v>9702</v>
@@ -1407,18 +1500,18 @@
         <v>15378</v>
       </c>
       <c r="K24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F25" s="5">
         <v>9792</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="1"/>
@@ -1429,18 +1522,18 @@
         <v>15450</v>
       </c>
       <c r="K25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E26" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="1"/>
@@ -1451,18 +1544,18 @@
         <v>15462</v>
       </c>
       <c r="K26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="1"/>
@@ -1473,18 +1566,18 @@
         <v>15486</v>
       </c>
       <c r="K27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E28" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="1"/>
@@ -1495,12 +1588,12 @@
         <v>15534</v>
       </c>
       <c r="K28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F29" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G29" s="5">
         <v>9959</v>
@@ -1514,18 +1607,18 @@
         <v>15834</v>
       </c>
       <c r="K29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="1"/>
@@ -1538,13 +1631,13 @@
     </row>
     <row r="31" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E31" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>98</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="1"/>
@@ -1560,75 +1653,75 @@
         <v>3</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>73</v>
+        <v>192</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" ref="H32" si="5">HEX2DEC(G32)-HEX2DEC(F32)+1</f>
-        <v>2016</v>
+        <f t="shared" ref="H32:H34" si="5">HEX2DEC(G32)-HEX2DEC(F32)+1</f>
+        <v>130</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" ref="I32" si="6">HEX2DEC(G32)-HEX2DEC(F$7)+1</f>
-        <v>18204</v>
+        <f t="shared" ref="I32:I34" si="6">HEX2DEC(G32)-HEX2DEC(F$7)+1</f>
+        <v>16318</v>
       </c>
     </row>
     <row r="33" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E33" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H33" s="8">
+      <c r="E33" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="5"/>
+        <v>392</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="6"/>
+        <v>16710</v>
+      </c>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="5"/>
+        <v>1495</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="6"/>
+        <v>18205</v>
+      </c>
+    </row>
+    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="8">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I33" s="8">
-        <f>HEX2DEC(G33)-HEX2DEC(F$7)+1</f>
+      <c r="I35" s="8">
+        <f>HEX2DEC(G35)-HEX2DEC(F$7)+1</f>
         <v>18237</v>
-      </c>
-    </row>
-    <row r="34" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="1"/>
-        <v>349</v>
-      </c>
-      <c r="I34" s="2">
-        <f>HEX2DEC(G34)-HEX2DEC(F$7)+1</f>
-        <v>18586</v>
-      </c>
-    </row>
-    <row r="35" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E35" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="I35" s="2">
-        <f>HEX2DEC(G35)-HEX2DEC(F$7)+1</f>
-        <v>18487</v>
       </c>
     </row>
     <row r="36" spans="5:14" x14ac:dyDescent="0.25">
@@ -1636,29 +1729,29 @@
         <v>3</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="G36" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>349</v>
+      </c>
+      <c r="I36" s="2">
+        <f>HEX2DEC(G36)-HEX2DEC(F$7)+1</f>
+        <v>18586</v>
+      </c>
+    </row>
+    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E37" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="H36" s="2">
-        <f t="shared" ref="H36" si="7">HEX2DEC(G36)-HEX2DEC(F36)+1</f>
-        <v>99</v>
-      </c>
-      <c r="I36" s="2">
-        <f t="shared" ref="I36" si="8">HEX2DEC(G36)-HEX2DEC(F$7)+1</f>
-        <v>18586</v>
-      </c>
-    </row>
-    <row r="37" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E37" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>92</v>
+      <c r="F37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="1"/>
@@ -1666,7 +1759,7 @@
       </c>
       <c r="I37" s="2">
         <f>HEX2DEC(G37)-HEX2DEC(F$7)+1</f>
-        <v>18602</v>
+        <v>18487</v>
       </c>
     </row>
     <row r="38" spans="5:14" x14ac:dyDescent="0.25">
@@ -1674,29 +1767,29 @@
         <v>3</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" ref="H38" si="7">HEX2DEC(G38)-HEX2DEC(F38)+1</f>
+        <v>99</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" ref="I38" si="8">HEX2DEC(G38)-HEX2DEC(F$7)+1</f>
+        <v>18586</v>
+      </c>
+    </row>
+    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="H38" s="2">
-        <f t="shared" ref="H38" si="9">HEX2DEC(G38)-HEX2DEC(F38)+1</f>
-        <v>723</v>
-      </c>
-      <c r="I38" s="2">
-        <f t="shared" ref="I38" si="10">HEX2DEC(G38)-HEX2DEC(F$7)+1</f>
-        <v>19325</v>
-      </c>
-    </row>
-    <row r="39" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>87</v>
+      <c r="F39" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="1"/>
@@ -1704,7 +1797,7 @@
       </c>
       <c r="I39" s="2">
         <f>HEX2DEC(G39)-HEX2DEC(F$7)+1</f>
-        <v>19341</v>
+        <v>18602</v>
       </c>
     </row>
     <row r="40" spans="5:14" x14ac:dyDescent="0.25">
@@ -1712,37 +1805,37 @@
         <v>3</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" ref="H40" si="11">HEX2DEC(G40)-HEX2DEC(F40)+1</f>
-        <v>235</v>
+        <f t="shared" ref="H40" si="9">HEX2DEC(G40)-HEX2DEC(F40)+1</f>
+        <v>723</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" ref="I40" si="12">HEX2DEC(G40)-HEX2DEC(F$7)+1</f>
-        <v>19576</v>
+        <f t="shared" ref="I40" si="10">HEX2DEC(G40)-HEX2DEC(F$7)+1</f>
+        <v>19325</v>
       </c>
     </row>
     <row r="41" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E41" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>74</v>
+        <v>10</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>16</v>
       </c>
       <c r="I41" s="2">
         <f>HEX2DEC(G41)-HEX2DEC(F$7)+1</f>
-        <v>19672</v>
+        <v>19341</v>
       </c>
     </row>
     <row r="42" spans="5:14" x14ac:dyDescent="0.25">
@@ -1750,37 +1843,37 @@
         <v>3</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="1"/>
-        <v>1055</v>
+        <f t="shared" ref="H42" si="11">HEX2DEC(G42)-HEX2DEC(F42)+1</f>
+        <v>235</v>
       </c>
       <c r="I42" s="2">
-        <f>HEX2DEC(G42)-HEX2DEC(F$7)+1</f>
-        <v>20727</v>
+        <f t="shared" ref="I42" si="12">HEX2DEC(G42)-HEX2DEC(F$7)+1</f>
+        <v>19576</v>
       </c>
     </row>
     <row r="43" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E43" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>83</v>
+      <c r="E43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="I43" s="2">
         <f>HEX2DEC(G43)-HEX2DEC(F$7)+1</f>
-        <v>20871</v>
+        <v>19672</v>
       </c>
     </row>
     <row r="44" spans="5:14" x14ac:dyDescent="0.25">
@@ -1788,317 +1881,561 @@
         <v>3</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" ref="H44" si="13">HEX2DEC(G44)-HEX2DEC(F44)+1</f>
-        <v>4733</v>
+        <f t="shared" si="1"/>
+        <v>1055</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" ref="I44" si="14">HEX2DEC(G44)-HEX2DEC(F$7)+1</f>
-        <v>25604</v>
-      </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="2"/>
+        <f>HEX2DEC(G44)-HEX2DEC(F$7)+1</f>
+        <v>20727</v>
+      </c>
     </row>
     <row r="45" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
-        <v>50</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>52</v>
+      <c r="E45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="1"/>
-        <v>394</v>
+        <v>144</v>
       </c>
       <c r="I45" s="2">
         <f>HEX2DEC(G45)-HEX2DEC(F$7)+1</f>
-        <v>25998</v>
-      </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="2"/>
+        <v>20871</v>
+      </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>24</v>
+      <c r="E46" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" ref="H46:H56" si="15">HEX2DEC(G46)-HEX2DEC(F46)+1</f>
-        <v>614</v>
+        <f t="shared" ref="H46" si="13">HEX2DEC(G46)-HEX2DEC(F46)+1</f>
+        <v>3936</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" ref="I46:I56" si="16">HEX2DEC(G46)-HEX2DEC(F$7)+1</f>
-        <v>26612</v>
+        <f t="shared" ref="I46" si="14">HEX2DEC(G46)-HEX2DEC(F$7)+1</f>
+        <v>24807</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>54</v>
+      <c r="E47" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>194</v>
       </c>
       <c r="H47" s="2">
+        <f t="shared" ref="H47:H51" si="15">HEX2DEC(G47)-HEX2DEC(F47)+1</f>
+        <v>193</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" ref="I47:I51" si="16">HEX2DEC(G47)-HEX2DEC(F$7)+1</f>
+        <v>25000</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E48" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="16"/>
+        <v>25011</v>
+      </c>
+      <c r="M48" s="1"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E49" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H49" s="2">
         <f t="shared" si="15"/>
         <v>18</v>
       </c>
-      <c r="I47" s="2">
-        <f t="shared" si="16"/>
-        <v>26630</v>
-      </c>
-      <c r="M47" s="1"/>
-      <c r="N47" s="2"/>
-    </row>
-    <row r="48" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
-        <v>56</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="15"/>
-        <v>6</v>
-      </c>
-      <c r="I48" s="2">
-        <f t="shared" si="16"/>
-        <v>26636</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E49" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="15"/>
-        <v>4890</v>
-      </c>
       <c r="I49" s="2">
         <f t="shared" si="16"/>
-        <v>31526</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+        <v>25029</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E50" s="4" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>59</v>
+        <v>174</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="15"/>
-        <v>96</v>
+        <f t="shared" ref="H50" si="17">HEX2DEC(G50)-HEX2DEC(F50)+1</f>
+        <v>12</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="16"/>
-        <v>31622</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>28</v>
+        <f t="shared" ref="I50" si="18">HEX2DEC(G50)-HEX2DEC(F$7)+1</f>
+        <v>25041</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E51" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="15"/>
-        <v>1382</v>
+        <v>129</v>
       </c>
       <c r="I51" s="2">
         <f t="shared" si="16"/>
+        <v>25170</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E52" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" ref="H52:H55" si="19">HEX2DEC(G52)-HEX2DEC(F52)+1</f>
+        <v>244</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" ref="I52:I55" si="20">HEX2DEC(G52)-HEX2DEC(F$7)+1</f>
+        <v>25414</v>
+      </c>
+      <c r="M52" s="1"/>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E53" s="4"/>
+      <c r="F53" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="20"/>
+        <v>25420</v>
+      </c>
+      <c r="M53" s="1"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E54" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="19"/>
+        <v>18</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="20"/>
+        <v>25438</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E55" s="4"/>
+      <c r="F55" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="19"/>
+        <v>42</v>
+      </c>
+      <c r="I55" s="2">
+        <f t="shared" si="20"/>
+        <v>25480</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="2"/>
+    </row>
+    <row r="56" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E56" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" ref="H56" si="21">HEX2DEC(G56)-HEX2DEC(F56)+1</f>
+        <v>124</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" ref="I56" si="22">HEX2DEC(G56)-HEX2DEC(F$7)+1</f>
+        <v>25604</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="2"/>
+    </row>
+    <row r="57" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="1"/>
+        <v>394</v>
+      </c>
+      <c r="I57" s="2">
+        <f>HEX2DEC(G57)-HEX2DEC(F$7)+1</f>
+        <v>25998</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" ref="H58:H68" si="23">HEX2DEC(G58)-HEX2DEC(F58)+1</f>
+        <v>614</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" ref="I58:I68" si="24">HEX2DEC(G58)-HEX2DEC(F$7)+1</f>
+        <v>26612</v>
+      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="23"/>
+        <v>18</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="24"/>
+        <v>26630</v>
+      </c>
+      <c r="M59" s="1"/>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="23"/>
+        <v>6</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="24"/>
+        <v>26636</v>
+      </c>
+    </row>
+    <row r="61" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="23"/>
+        <v>4890</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="24"/>
+        <v>31526</v>
+      </c>
+    </row>
+    <row r="62" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E62" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="23"/>
+        <v>96</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="24"/>
+        <v>31622</v>
+      </c>
+    </row>
+    <row r="63" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>21</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="23"/>
+        <v>1382</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="24"/>
         <v>33004</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E52" s="4" t="s">
+    <row r="64" spans="5:14" x14ac:dyDescent="0.25">
+      <c r="E64" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G64" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="H64" s="2">
+        <f t="shared" si="23"/>
+        <v>384</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="24"/>
+        <v>33388</v>
+      </c>
+      <c r="K64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F65" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G65" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="23"/>
+        <v>512</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="24"/>
+        <v>33900</v>
+      </c>
+      <c r="K65" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F66" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H52" s="2">
-        <f t="shared" si="15"/>
-        <v>384</v>
-      </c>
-      <c r="I52" s="2">
-        <f t="shared" si="16"/>
-        <v>33388</v>
-      </c>
-      <c r="K52" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F53" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G53" s="5" t="s">
+      <c r="G66" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" si="23"/>
+        <v>512</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="24"/>
+        <v>34412</v>
+      </c>
+      <c r="J66" s="2"/>
+      <c r="K66" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="2">
-        <f t="shared" si="15"/>
-        <v>512</v>
-      </c>
-      <c r="I53" s="2">
-        <f t="shared" si="16"/>
-        <v>33900</v>
-      </c>
-      <c r="K53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F54" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G54" s="5" t="s">
+      <c r="H67" s="2">
+        <f t="shared" si="23"/>
+        <v>1412</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="24"/>
+        <v>35824</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="23"/>
+        <v>1216</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="24"/>
+        <v>37040</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F69" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H54" s="2">
-        <f t="shared" si="15"/>
-        <v>512</v>
-      </c>
-      <c r="I54" s="2">
-        <f t="shared" si="16"/>
-        <v>34412</v>
-      </c>
-      <c r="J54" s="2"/>
-      <c r="K54" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H55" s="2">
-        <f t="shared" si="15"/>
-        <v>1412</v>
-      </c>
-      <c r="I55" s="2">
-        <f t="shared" si="16"/>
-        <v>35824</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H56" s="2">
-        <f t="shared" si="15"/>
-        <v>1216</v>
-      </c>
-      <c r="I56" s="2">
-        <f t="shared" si="16"/>
-        <v>37040</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F57" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H57" s="2">
-        <f t="shared" ref="H57:H58" si="17">HEX2DEC(G57)-HEX2DEC(F57)+1</f>
+      <c r="G69" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" ref="H69:H70" si="25">HEX2DEC(G69)-HEX2DEC(F69)+1</f>
         <v>4904</v>
       </c>
-      <c r="I57" s="2">
-        <f t="shared" ref="I57:I58" si="18">HEX2DEC(G57)-HEX2DEC(F$7)+1</f>
+      <c r="I69" s="2">
+        <f t="shared" ref="I69:I70" si="26">HEX2DEC(G69)-HEX2DEC(F$7)+1</f>
         <v>41944</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="2">
-        <f>HEX2DEC(B58)-HEX2DEC(A58)+1</f>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="2">
+        <f>HEX2DEC(B70)-HEX2DEC(A70)+1</f>
         <v>168</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D70" t="s">
+        <v>122</v>
+      </c>
+      <c r="E70" t="s">
+        <v>122</v>
+      </c>
+      <c r="F70" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E58" t="s">
-        <v>125</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H58" s="2">
-        <f t="shared" si="17"/>
+      <c r="G70" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" si="25"/>
         <v>168</v>
       </c>
-      <c r="I58" s="2">
-        <f t="shared" si="18"/>
+      <c r="I70" s="2">
+        <f t="shared" si="26"/>
         <v>42112</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E62" s="3"/>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E74" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="E2:I54" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="E2:I66" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -2108,7 +2445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342D484E-E4B6-4114-83F0-3D06829355AA}">
   <dimension ref="A2:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2120,51 +2457,51 @@
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" t="s">
         <v>150</v>
       </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>151</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>152</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>153</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>154</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>155</v>
       </c>
-      <c r="H2" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J2" t="s">
-        <v>158</v>
-      </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B3" s="5">
         <v>9702</v>
@@ -2186,7 +2523,7 @@
         <v>112</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2209,7 +2546,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B4" t="str">
         <f>DEC2HEX(HEX2DEC(B3)+12)</f>
@@ -2232,7 +2569,7 @@
         <v>131</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I4">
         <v>208</v>
@@ -2255,10 +2592,10 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" ref="B5:B15" si="0">DEC2HEX(HEX2DEC(B4)+12)</f>
+        <f t="shared" ref="B5:B14" si="0">DEC2HEX(HEX2DEC(B4)+12)</f>
         <v>971A</v>
       </c>
       <c r="C5">
@@ -2278,7 +2615,7 @@
         <v>63</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I5">
         <v>48</v>
@@ -2301,7 +2638,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
@@ -2324,7 +2661,7 @@
         <v>131</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I6">
         <v>208</v>
@@ -2347,7 +2684,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
@@ -2370,7 +2707,7 @@
         <v>63</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I7">
         <v>48</v>
@@ -2393,7 +2730,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -2415,7 +2752,7 @@
         <v>80</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -2438,7 +2775,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -2460,7 +2797,7 @@
         <v>80</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -2483,7 +2820,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -2505,7 +2842,7 @@
         <v>78</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I10">
         <v>253</v>
@@ -2528,7 +2865,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -2573,7 +2910,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -2595,7 +2932,7 @@
         <v>63</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I12">
         <v>192</v>
@@ -2618,7 +2955,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -2640,7 +2977,7 @@
         <v>135</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I13">
         <v>224</v>
@@ -2663,7 +3000,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -2685,7 +3022,7 @@
         <v>135</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I14">
         <v>0</v>

</xml_diff>